<commit_message>
changes for assignment 2
changes processing file, processeddata, and eda files
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69F5804-BD14-4B61-9695-C3202B904432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52FD056-1FD2-4252-BDB4-BA2382D02F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3984" yWindow="1284" windowWidth="17280" windowHeight="10656" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,15 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
   <si>
     <t>Height</t>
   </si>
   <si>
     <t>Weight</t>
-  </si>
-  <si>
-    <t>sixty</t>
   </si>
   <si>
     <t>M</t>
@@ -442,16 +439,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -459,16 +456,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>180</v>
       </c>
@@ -476,16 +473,16 @@
         <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>24.7</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>175</v>
       </c>
@@ -493,33 +490,33 @@
         <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>22.9</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>60</v>
       </c>
       <c r="B4">
         <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>23.4</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>178</v>
       </c>
@@ -527,16 +524,16 @@
         <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>192</v>
       </c>
@@ -544,16 +541,16 @@
         <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <v>24.4</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -561,16 +558,16 @@
         <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>15.9</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>156</v>
       </c>
@@ -578,16 +575,16 @@
         <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>166</v>
       </c>
@@ -595,16 +592,16 @@
         <v>110</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9">
         <v>39.9</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>155</v>
       </c>
@@ -612,16 +609,16 @@
         <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10">
         <v>22.5</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>145</v>
       </c>
@@ -629,30 +626,33 @@
         <v>7000</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11">
         <v>33.299999999999997</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>165</v>
       </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D12">
         <v>18.399999999999999</v>
       </c>
       <c r="E12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>133</v>
       </c>
@@ -660,16 +660,16 @@
         <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13">
         <v>25.4</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>166</v>
       </c>
@@ -677,16 +677,16 @@
         <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14">
         <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>154</v>
       </c>
@@ -694,13 +694,13 @@
         <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <v>21.1</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -712,81 +712,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A2C8F0-62B4-4D60-B490-D490A3E0B40F}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
-    <col min="3" max="3" width="54.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="54.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>